<commit_message>
Archivos principales en proyecto integrador
</commit_message>
<xml_diff>
--- a/CASO-VENTAS-PARA-TODOS.xlsx
+++ b/CASO-VENTAS-PARA-TODOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAVIDMP 2021\CURSOS 2021-1\GU-Fundamentos de Programacion\PROYECTO INTEGRADOR\CASOS\Grupo 2\G-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DESARROLLO CLASES FP\FP-2021-G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Productos</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>netoTotal</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>IdDNI</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>Pera</t>
   </si>
 </sst>
 </file>
@@ -171,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -270,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -293,6 +317,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N36"/>
+  <dimension ref="B3:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,13 +744,27 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>20</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -789,7 +837,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>2</v>
       </c>
@@ -813,7 +861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
@@ -841,8 +889,14 @@
         <f>SUM(J30:J31)</f>
         <v>101.75999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="14"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,8 +909,20 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="F20" s="1"/>
@@ -865,8 +931,12 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="F21" s="1"/>
@@ -875,8 +945,12 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="F22" s="1"/>
@@ -885,8 +959,12 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="F23" s="1"/>
@@ -895,8 +973,12 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="F24" s="1"/>
@@ -905,16 +987,34 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D28" s="11" t="s">
         <v>32</v>
       </c>
@@ -924,8 +1024,12 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
         <v>33</v>
       </c>
@@ -947,8 +1051,12 @@
       <c r="J29" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>35</v>
       </c>
@@ -972,8 +1080,12 @@
         <f>I30*G30</f>
         <v>93.6</v>
       </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>38</v>
       </c>
@@ -997,8 +1109,12 @@
         <f>G31*I31</f>
         <v>8.16</v>
       </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1044,7 +1160,8 @@
       <c r="J36" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="N18:Q18"/>
     <mergeCell ref="F16:K16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B4:H4"/>

</xml_diff>